<commit_message>
added EFPIA event recording
</commit_message>
<xml_diff>
--- a/data/conferences.xlsx
+++ b/data/conferences.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="299">
   <si>
     <t>Conference</t>
   </si>
@@ -915,6 +915,9 @@
   <si>
     <t>Bringing estimands to lifelifethrough real case studies through real case studies</t>
   </si>
+  <si>
+    <t>https://www.psiweb.org/vod/item/psi-eiwg-webinar-estimands-in-oncology---how-and-why</t>
+  </si>
 </sst>
 </file>
 
@@ -1403,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AB30" sqref="AB30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="255.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,7 +3521,9 @@
       <c r="AA30" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="AB30" s="6"/>
+      <c r="AB30" s="6" t="s">
+        <v>298</v>
+      </c>
       <c r="AC30" s="6"/>
       <c r="AD30" s="6"/>
       <c r="AE30" s="6"/>
@@ -44967,10 +44972,11 @@
     <hyperlink ref="M25" r:id="rId21"/>
     <hyperlink ref="D29" r:id="rId22"/>
     <hyperlink ref="D30" r:id="rId23"/>
+    <hyperlink ref="AB30" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
-  <drawing r:id="rId25"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>